<commit_message>
Add short demo 06_pandas_demo.py and sample file People.xlsx for pandas library
</commit_message>
<xml_diff>
--- a/13_File_Handling_Lab_27_01_2026/People.xlsx
+++ b/13_File_Handling_Lab_27_01_2026/People.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -378,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -424,6 +424,14 @@
       </c>
       <c r="B5" s="1">
         <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>